<commit_message>
Final ML Model, Predictions and Feature Extraction Added
</commit_message>
<xml_diff>
--- a/Training/CSV Files/feature_data.xlsx
+++ b/Training/CSV Files/feature_data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anushka\Projects\Google Girl Hackathon\Training\CSV Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE24C2B7-9A5D-4A0F-BF5D-CCFF6508F177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -52,6 +46,39 @@
     <t>IP6S.v</t>
   </si>
   <si>
+    <t>c1355.v</t>
+  </si>
+  <si>
+    <t>c17.v</t>
+  </si>
+  <si>
+    <t>c1908.v</t>
+  </si>
+  <si>
+    <t>c2670.v</t>
+  </si>
+  <si>
+    <t>c3540.v</t>
+  </si>
+  <si>
+    <t>c432.v</t>
+  </si>
+  <si>
+    <t>c499.v</t>
+  </si>
+  <si>
+    <t>c5315.v</t>
+  </si>
+  <si>
+    <t>c6288.v</t>
+  </si>
+  <si>
+    <t>c7552.v</t>
+  </si>
+  <si>
+    <t>c880.v</t>
+  </si>
+  <si>
     <t>s1238.v</t>
   </si>
   <si>
@@ -97,56 +124,23 @@
     <t>s9234.v</t>
   </si>
   <si>
-    <t>c1355.v</t>
-  </si>
-  <si>
-    <t>c17.v</t>
-  </si>
-  <si>
-    <t>c1908.v</t>
-  </si>
-  <si>
-    <t>c2670.v</t>
-  </si>
-  <si>
-    <t>c3540.v</t>
-  </si>
-  <si>
-    <t>c432.v</t>
-  </si>
-  <si>
-    <t>c499.v</t>
-  </si>
-  <si>
-    <t>c5315.v</t>
-  </si>
-  <si>
-    <t>c6288.v</t>
-  </si>
-  <si>
-    <t>c7552.v</t>
-  </si>
-  <si>
-    <t>c880.v</t>
-  </si>
-  <si>
     <t>Combinational</t>
   </si>
   <si>
     <t>Sequential</t>
   </si>
   <si>
+    <t>ISCAS85</t>
+  </si>
+  <si>
     <t>ISCAS89</t>
-  </si>
-  <si>
-    <t>ISCAS85</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,18 +157,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD3D3D3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -206,372 +194,22 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6666"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:v>Depth</c:v>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Features!$A$2:$A$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>961</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5787</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>997</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1284</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7321</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>24408</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>239</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>18558</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>24951</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2437</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>267</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>337</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4401</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>992</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1059</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1559</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2226</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>296</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>368</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3492</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4768</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4734</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Features!$D$2:$D$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3375-413E-86BA-64F3B013DD1F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="50010001"/>
-        <c:axId val="50010002"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="50010001"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010002"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="50010002"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010001"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -609,7 +247,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -643,7 +281,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -678,10 +315,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -854,22 +490,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" customWidth="1"/>
-    <col min="3" max="3" width="21.6640625" customWidth="1"/>
-    <col min="4" max="5" width="20.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="28.5546875" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -892,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>4</v>
       </c>
@@ -906,7 +534,7 @@
         <v>2</v>
       </c>
       <c r="E2">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -915,7 +543,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>4</v>
       </c>
@@ -929,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -938,7 +566,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>13</v>
       </c>
@@ -949,10 +577,10 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -961,21 +589,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5">
-        <v>961</v>
+        <v>992</v>
       </c>
       <c r="B5">
-        <v>961</v>
+        <v>992</v>
       </c>
       <c r="C5">
-        <v>428</v>
+        <v>474</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>96.1</v>
+        <v>47.4</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -984,21 +612,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6">
-        <v>5787</v>
+        <v>12</v>
       </c>
       <c r="B6">
-        <v>5787</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>2573</v>
+        <v>6</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6">
-        <v>578.70000000000005</v>
+        <v>0.6</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -1007,21 +635,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7">
-        <v>997</v>
+        <v>1059</v>
       </c>
       <c r="B7">
-        <v>997</v>
+        <v>1059</v>
       </c>
       <c r="C7">
-        <v>490</v>
+        <v>441</v>
       </c>
       <c r="D7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E7">
-        <v>99.7</v>
+        <v>44.1</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -1030,21 +658,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8">
-        <v>1284</v>
+        <v>1559</v>
       </c>
       <c r="B8">
-        <v>1284</v>
+        <v>1559</v>
       </c>
       <c r="C8">
-        <v>550</v>
+        <v>676</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E8">
-        <v>128.4</v>
+        <v>67.59999999999999</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
@@ -1053,21 +681,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9">
-        <v>7321</v>
+        <v>2226</v>
       </c>
       <c r="B9">
-        <v>7321</v>
+        <v>2226</v>
       </c>
       <c r="C9">
-        <v>3448</v>
+        <v>956</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E9">
-        <v>732.1</v>
+        <v>95.59999999999999</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -1076,21 +704,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10">
-        <v>16</v>
+        <v>296</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>296</v>
       </c>
       <c r="C10">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10">
-        <v>1.6</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1099,21 +727,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11">
-        <v>24408</v>
+        <v>368</v>
       </c>
       <c r="B11">
-        <v>24408</v>
+        <v>368</v>
       </c>
       <c r="C11">
-        <v>12204</v>
+        <v>162</v>
       </c>
       <c r="D11">
         <v>2</v>
       </c>
       <c r="E11">
-        <v>2440.8000000000002</v>
+        <v>16.2</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -1122,21 +750,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12">
-        <v>239</v>
+        <v>3492</v>
       </c>
       <c r="B12">
-        <v>239</v>
+        <v>3492</v>
       </c>
       <c r="C12">
-        <v>97</v>
+        <v>1413</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="E12">
-        <v>23.9</v>
+        <v>141.3</v>
       </c>
       <c r="F12" t="s">
         <v>17</v>
@@ -1145,21 +773,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13">
-        <v>18558</v>
+        <v>4768</v>
       </c>
       <c r="B13">
-        <v>18558</v>
+        <v>4768</v>
       </c>
       <c r="C13">
-        <v>8709</v>
+        <v>2384</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E13">
-        <v>1855.8</v>
+        <v>238.4</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
@@ -1168,21 +796,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14">
-        <v>24951</v>
+        <v>4734</v>
       </c>
       <c r="B14">
-        <v>24951</v>
+        <v>4734</v>
       </c>
       <c r="C14">
-        <v>11448</v>
+        <v>2102</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E14">
-        <v>2495.1</v>
+        <v>210.2</v>
       </c>
       <c r="F14" t="s">
         <v>19</v>
@@ -1191,21 +819,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15">
-        <v>305</v>
+        <v>640</v>
       </c>
       <c r="B15">
-        <v>305</v>
+        <v>640</v>
       </c>
       <c r="C15">
-        <v>140</v>
+        <v>294</v>
       </c>
       <c r="D15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>30.5</v>
+        <v>29.4</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
@@ -1214,113 +842,113 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16">
-        <v>2437</v>
+        <v>961</v>
       </c>
       <c r="B16">
-        <v>2437</v>
+        <v>961</v>
       </c>
       <c r="C16">
-        <v>1004</v>
+        <v>428</v>
       </c>
       <c r="D16">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>243.7</v>
+        <v>42.8</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
-        <v>267</v>
+        <v>5787</v>
       </c>
       <c r="B17">
-        <v>267</v>
+        <v>5787</v>
       </c>
       <c r="C17">
-        <v>107</v>
+        <v>2573</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E17">
-        <v>26.7</v>
+        <v>257.3</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
       </c>
       <c r="G17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18">
-        <v>337</v>
+        <v>997</v>
       </c>
       <c r="B18">
-        <v>337</v>
+        <v>997</v>
       </c>
       <c r="C18">
-        <v>139</v>
+        <v>490</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E18">
-        <v>33.700000000000003</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19">
-        <v>4401</v>
+        <v>1284</v>
       </c>
       <c r="B19">
-        <v>4401</v>
+        <v>1284</v>
       </c>
       <c r="C19">
-        <v>2027</v>
+        <v>550</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>440.1</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s">
         <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20">
-        <v>992</v>
+        <v>7321</v>
       </c>
       <c r="B20">
-        <v>992</v>
+        <v>7321</v>
       </c>
       <c r="C20">
-        <v>474</v>
+        <v>3448</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>99.2</v>
+        <v>344.8</v>
       </c>
       <c r="F20" t="s">
         <v>25</v>
@@ -1329,21 +957,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="F21" t="s">
         <v>26</v>
@@ -1352,21 +980,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22">
-        <v>1059</v>
+        <v>24408</v>
       </c>
       <c r="B22">
-        <v>1059</v>
+        <v>24408</v>
       </c>
       <c r="C22">
-        <v>441</v>
+        <v>12204</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E22">
-        <v>105.9</v>
+        <v>1220.4</v>
       </c>
       <c r="F22" t="s">
         <v>27</v>
@@ -1375,21 +1003,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23">
-        <v>1559</v>
+        <v>239</v>
       </c>
       <c r="B23">
-        <v>1559</v>
+        <v>239</v>
       </c>
       <c r="C23">
-        <v>676</v>
+        <v>97</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>155.9</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="F23" t="s">
         <v>28</v>
@@ -1398,21 +1026,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24">
-        <v>2226</v>
+        <v>18558</v>
       </c>
       <c r="B24">
-        <v>2226</v>
+        <v>18558</v>
       </c>
       <c r="C24">
-        <v>956</v>
+        <v>8709</v>
       </c>
       <c r="D24">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E24">
-        <v>222.6</v>
+        <v>870.9</v>
       </c>
       <c r="F24" t="s">
         <v>29</v>
@@ -1421,21 +1049,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25">
-        <v>296</v>
+        <v>24951</v>
       </c>
       <c r="B25">
-        <v>296</v>
+        <v>24951</v>
       </c>
       <c r="C25">
-        <v>120</v>
+        <v>11448</v>
       </c>
       <c r="D25">
         <v>9</v>
       </c>
       <c r="E25">
-        <v>29.6</v>
+        <v>1144.8</v>
       </c>
       <c r="F25" t="s">
         <v>30</v>
@@ -1444,21 +1072,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26">
-        <v>368</v>
+        <v>305</v>
       </c>
       <c r="B26">
-        <v>368</v>
+        <v>305</v>
       </c>
       <c r="C26">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E26">
-        <v>36.799999999999997</v>
+        <v>14</v>
       </c>
       <c r="F26" t="s">
         <v>31</v>
@@ -1467,21 +1095,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27">
-        <v>3492</v>
+        <v>2437</v>
       </c>
       <c r="B27">
-        <v>3492</v>
+        <v>2437</v>
       </c>
       <c r="C27">
-        <v>1413</v>
+        <v>1004</v>
       </c>
       <c r="D27">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E27">
-        <v>349.2</v>
+        <v>100.4</v>
       </c>
       <c r="F27" t="s">
         <v>32</v>
@@ -1490,21 +1118,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28">
-        <v>4768</v>
+        <v>267</v>
       </c>
       <c r="B28">
-        <v>4768</v>
+        <v>267</v>
       </c>
       <c r="C28">
-        <v>2384</v>
+        <v>107</v>
       </c>
       <c r="D28">
         <v>2</v>
       </c>
       <c r="E28">
-        <v>476.8</v>
+        <v>10.7</v>
       </c>
       <c r="F28" t="s">
         <v>33</v>
@@ -1513,21 +1141,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29">
-        <v>4734</v>
+        <v>337</v>
       </c>
       <c r="B29">
-        <v>4734</v>
+        <v>337</v>
       </c>
       <c r="C29">
-        <v>2102</v>
+        <v>139</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>473.4</v>
+        <v>13.9</v>
       </c>
       <c r="F29" t="s">
         <v>34</v>
@@ -1536,21 +1164,21 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30">
-        <v>640</v>
+        <v>4401</v>
       </c>
       <c r="B30">
-        <v>640</v>
+        <v>4401</v>
       </c>
       <c r="C30">
-        <v>294</v>
+        <v>2027</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>64</v>
+        <v>202.7</v>
       </c>
       <c r="F30" t="s">
         <v>35</v>
@@ -1560,27 +1188,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D100">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E100">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
-      <formula>10</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
-      <formula>5</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>